<commit_message>
feat add api qr code + fix l'interface messagerie
</commit_message>
<xml_diff>
--- a/src/main/resources/datasets/dataset.xlsx
+++ b/src/main/resources/datasets/dataset.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\Desktop\pidev\3A5_DevMasters\src\main\java\edu\esprit\services\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\Desktop\pidev\3A5_DevMasters\src\main\resources\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03874411-7970-47A4-B22A-0D6C01409120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4008E9A3-D445-4E82-9CCE-CF2B22334BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="104">
   <si>
     <t>bonjour</t>
   </si>
@@ -274,6 +274,72 @@
   </si>
   <si>
     <t>mech barcha kaad net3alem</t>
+  </si>
+  <si>
+    <t>iheb</t>
+  </si>
+  <si>
+    <t>c'est un prof tres intelligent dans le domaine IT et il est l'encadreur des autres équipes</t>
+  </si>
+  <si>
+    <t>kifeh nestaamel baladity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">baladity esta3melha sehel barcha jareb les fonctionnalités eli andna w ija koli </t>
+  </si>
+  <si>
+    <t>fama des evenements ?</t>
+  </si>
+  <si>
+    <t>ey tnajem tchouf les evenements eli mawjoudin l periode hedhy sehla yesser odkhel lel evenement hawka fel menu</t>
+  </si>
+  <si>
+    <t>kifeh n3ady reclamation</t>
+  </si>
+  <si>
+    <t>sehel barcha bech t3adi reclamation juste todkhel lel reclamation w takhtar type reclamation eli bech taadih w testana directeur yjewbouk al reclamation mte3ek</t>
+  </si>
+  <si>
+    <t>plus mta3 l application hedhy chneya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fama flous </t>
+  </si>
+  <si>
+    <t>le betbi3a caisse fergha</t>
+  </si>
+  <si>
+    <t>chnwa famma jdid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bech taaref chnwa famma jdid odkhel lel actualite talka kol chy sayer </t>
+  </si>
+  <si>
+    <t>tsahel alik l contact f kol baladeya</t>
+  </si>
+  <si>
+    <t>kifeh nhabet publicite</t>
+  </si>
+  <si>
+    <t>easy peasy taamer formlaire w tet3ada lel paiement wtkhales b soum ramzi w jawek foll</t>
+  </si>
+  <si>
+    <t>kadech tahky men lougha</t>
+  </si>
+  <si>
+    <t>je parle en francais,arabe,anglais</t>
+  </si>
+  <si>
+    <t>chneya loumour</t>
+  </si>
+  <si>
+    <t>famm chyy jdid</t>
+  </si>
+  <si>
+    <t>kadeh omrek</t>
+  </si>
+  <si>
+    <t>En tant que chatbot maandich reponse lel question mte3ek</t>
   </si>
 </sst>
 </file>
@@ -594,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -949,6 +1015,94 @@
         <v>81</v>
       </c>
     </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>91</v>
+      </c>
+      <c r="B49" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>93</v>
+      </c>
+      <c r="B50" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>96</v>
+      </c>
+      <c r="B51" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>98</v>
+      </c>
+      <c r="B52" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>100</v>
+      </c>
+      <c r="B53" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54" t="s">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>